<commit_message>
ui/ux improvements and minor bug fixes
</commit_message>
<xml_diff>
--- a/assets/Database.xlsx
+++ b/assets/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\65906\AndroidStudioProjects\calory_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B91D77-AD7D-4A46-81BE-72B4236EC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56B9302-9C1A-4F22-8C6C-E730EF346C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upperBodyData" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Pushups</t>
   </si>
   <si>
-    <t>Start in a straight arm plank position, with palm directly below the shoulders. Lower yourself until the elbows are 90 degrees, then push youself back up, ensuring the back is straight during the entire motion.</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -106,154 +103,157 @@
     <t>Squats</t>
   </si>
   <si>
-    <t>Stand straight with your feet shoulder width apart, lower yourself till the knees are 90 degrees before pushing yourself back up.</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
     <t>Split Squat</t>
   </si>
   <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Wall Squat</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>Squat Jump</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>Single-leg hip raise</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>Lunges</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>Jumping Jacks</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>Skaters</t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>Burpees</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Sit-up</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Plank</t>
+  </si>
+  <si>
+    <t>Lie down on your stomach and bring your body up with your elbows on the floor. Hold the position while keeping the back straight.</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Mountain Climbers</t>
+  </si>
+  <si>
+    <t>In a pushup position, bring the knees towards the chest for each rep.</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Single leg toe touch</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Leg raises</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>Crunches</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>Russian Twist</t>
+  </si>
+  <si>
+    <t>Sit on the floor with your knee slightly bent, interlace your fingers infront of your chest. Lean back 45 degrees while maintaining balance. For each rep use your abdominals to twist your upper body to the right, then back to center, and then to the left .</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Swim</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>Stand straight with your feet shoulder width apart. Lower yourself till the knees are 90 degrees before pushing yourself back up.</t>
+  </si>
+  <si>
     <t>Stand straight with one leg in front while the other behind. Lower yourself until both knees are 90 degrees before pushing yourself back up.</t>
   </si>
   <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>Wall Squat</t>
-  </si>
-  <si>
     <t>Lean against a wall will your legs slightly forward. Lower yourself until both knees are 90 degrees and hold the position.</t>
   </si>
   <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>Squat Jump</t>
-  </si>
-  <si>
-    <t>Stand straight with your feet shoulder width apart, lower yourself till the knees are 90 degrees before pushing youself back up with a jump.</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>Single-leg hip raise</t>
+    <t>Stand straight with your feet shoulder width apart. Lower yourself till the knees are 90 degrees before pushing youself back up with a jump.</t>
   </si>
   <si>
     <t>While lying down on your back, keep your feet close to your body. Lift up one leg and proceed to thrust the body upwards.</t>
   </si>
   <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>Lunges</t>
-  </si>
-  <si>
-    <t>Start of standing straight. Take a step forward and lower the body until both the knees are 90degrees before pushing youself back up to the original position</t>
-  </si>
-  <si>
-    <t>L7</t>
-  </si>
-  <si>
-    <t>Jumping Jacks</t>
-  </si>
-  <si>
-    <t>L8</t>
-  </si>
-  <si>
-    <t>Skaters</t>
-  </si>
-  <si>
-    <t>L9</t>
-  </si>
-  <si>
-    <t>Burpees</t>
-  </si>
-  <si>
-    <t>Start off standing straight, do a squat and place ur palms on the floor. Proceed to kick out both your legs to transition into a pushup position, before jumping back into a squat before standing back up.</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>Sit-up</t>
-  </si>
-  <si>
-    <t>Lie down on your back, bringing the feet close to the body. With your palms on your ears, bring up your upper body so that your elbows touch your knees, before lowering youself back.</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>Plank</t>
-  </si>
-  <si>
-    <t>Lie down on your stomach and bring your body up with your elbows on the floor. Hold the position while keeping the back straight.</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>Mountain Climbers</t>
-  </si>
-  <si>
-    <t>In a pushup position, bring the knees towards the chest for each rep.</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>Single leg toe touch</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>Leg raises</t>
-  </si>
-  <si>
-    <t>Lie down on your back and bring both feet up.For each rep, bring the legs up until they are perpendicular to the floor, while keeping them as straight as possible before lowering.</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>Crunches</t>
-  </si>
-  <si>
-    <t>Lie down on your back, bring your feet up until your lower half of the legs are parallel to the floor. With your palms on your ears, bring up your upper body so that your elbows touch your knees, before lowering youself back.</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>Russian Twist</t>
-  </si>
-  <si>
-    <t>Sit on the floor with your knee slightly bent, interlace your fingers infront of your chest. Lean back 45 degrees while maintaining balance. For each rep use your abdominals to twist your upper body to the right, then back to center, and then to the left .</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Swim</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>Cycle</t>
-  </si>
-  <si>
-    <t>Nil</t>
+    <t>Start off standing straight, do a squat and place ur palms on the floor. Proceed to kick out both your legs to transition into a pushup position. Jump back into a squat before standing back up.</t>
+  </si>
+  <si>
+    <t>Start of standing straight. Take a step forward and lower the body until both the knees are 90degrees. Push youself back up to the original position.</t>
+  </si>
+  <si>
+    <t>Start in a straight arm plank position, with palm directly below the shoulders. Lower yourself until the elbows are 90 degrees. Push youself back up, ensuring the back is straight during the entire motion.</t>
+  </si>
+  <si>
+    <t>Lie down on your back, bringing the feet close to the body. With your palms on your ears, bring up your upper body so that your elbows touch your knees.  Lower youself back down, with your back touching the floor.</t>
+  </si>
+  <si>
+    <t>Lie down on your back and bring both feet up. For each rep, bring the legs up until they are perpendicular to the floor. Keep your arms as straight as possible before lowering.</t>
+  </si>
+  <si>
+    <t>Lie down on your back, bring your feet up until your lower half of the legs are parallel to the floor. With your palms on your ears, bring up your upper body so that your elbows touch your knees. Lower youself back down, with your back touching the floor.</t>
   </si>
 </sst>
 </file>
@@ -540,14 +540,14 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="129.5703125" customWidth="1"/>
+    <col min="5" max="5" width="176.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -581,12 +581,12 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>30</v>
@@ -595,15 +595,15 @@
         <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>60</v>
@@ -612,15 +612,15 @@
         <v>60</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>40</v>
@@ -629,15 +629,15 @@
         <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
         <v>60</v>
@@ -646,15 +646,15 @@
         <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
         <v>40</v>
@@ -663,15 +663,15 @@
         <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>60</v>
@@ -680,10 +680,10 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3674,14 +3674,14 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="131.85546875" customWidth="1"/>
+    <col min="5" max="5" width="170.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3703,7 +3703,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>60</v>
@@ -3712,15 +3712,15 @@
         <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>60</v>
@@ -3729,30 +3729,30 @@
         <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
@@ -3761,15 +3761,15 @@
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -3778,15 +3778,15 @@
         <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1">
         <v>30</v>
@@ -3795,15 +3795,15 @@
         <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1">
         <v>30</v>
@@ -3812,15 +3812,15 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>20</v>
@@ -3829,15 +3829,15 @@
         <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>30</v>
@@ -3846,10 +3846,10 @@
         <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3864,15 +3864,15 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="155.42578125" customWidth="1"/>
+    <col min="5" max="5" width="213.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3894,7 +3894,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1">
         <v>60</v>
@@ -3903,29 +3903,29 @@
         <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1">
         <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>30</v>
@@ -3934,15 +3934,15 @@
         <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -3951,15 +3951,15 @@
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1">
         <v>40</v>
@@ -3968,15 +3968,15 @@
         <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
         <v>60</v>
@@ -3985,15 +3985,15 @@
         <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1">
         <v>40</v>
@@ -4002,10 +4002,10 @@
         <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7024,44 +7024,44 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1">
         <v>1800</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>1800</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1">
         <v>1800</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>